<commit_message>
full rerun of figs
</commit_message>
<xml_diff>
--- a/tables/monthly_tables/nondetrended_covar/explained_var_ratio.xlsx
+++ b/tables/monthly_tables/nondetrended_covar/explained_var_ratio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A43"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,215 +439,1656 @@
           <t>1</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>0.1093680188059807</v>
       </c>
+      <c r="B2" t="n">
+        <v>0.09274386614561081</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.117696613073349</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1147505342960358</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.1355419605970383</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.198231041431427</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.2297586649656296</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.1531559973955154</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.09801967442035675</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.1574626863002777</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.09306417405605316</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.1140516474843025</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>0.07749371975660324</v>
       </c>
+      <c r="B3" t="n">
+        <v>0.07743401080369949</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.06877364963293076</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.08067106455564499</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.06899027526378632</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.07616633176803589</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.1234550476074219</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.07356687635183334</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.06852183490991592</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.05621287226676941</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0683695450425148</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.07097554206848145</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>0.06218824908137321</v>
       </c>
+      <c r="B4" t="n">
+        <v>0.05229384079575539</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.06729238480329514</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.06434258818626404</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.05062343180179596</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.06175826489925385</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.07915123552083969</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0670073926448822</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.06133376806974411</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.04852304607629776</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.06006099283695221</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.05333355069160461</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>0.05281843245029449</v>
       </c>
+      <c r="B5" t="n">
+        <v>0.04950251057744026</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.05351328477263451</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.05439808964729309</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.04904606938362122</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.05416468158364296</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.06967274844646454</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.06387048214673996</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.05015856400132179</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.04408428072929382</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.05421240255236626</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.04991744458675385</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>0.04702460765838623</v>
       </c>
+      <c r="B6" t="n">
+        <v>0.0419447124004364</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.04929415509104729</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.04662769287824631</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.04533115029335022</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.04257034882903099</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.06235538795590401</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.06010306254029274</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.04965679720044136</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.04037827625870705</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.04628706350922585</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.04785268008708954</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>0.03959570452570915</v>
       </c>
+      <c r="B7" t="n">
+        <v>0.03673277422785759</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.04189349710941315</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.04253917187452316</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.03969820216298103</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0388290137052536</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.05856871232390404</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.05050433427095413</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.0449686273932457</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.03655165061354637</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.04036521911621094</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.042680773884058</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>0.03446648269891739</v>
       </c>
+      <c r="B8" t="n">
+        <v>0.03609712421894073</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.04006700962781906</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.03838459402322769</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.03676043450832367</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.03803860768675804</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.03578697517514229</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.04623236507177353</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.03987497091293335</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.03519820049405098</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.03659946098923683</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.04139972105622292</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>0.03123152256011963</v>
       </c>
+      <c r="B9" t="n">
+        <v>0.03414048999547958</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.03738147392868996</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.03315179422497749</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.03385865688323975</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.03455705568194389</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.02877422980964184</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.0416281558573246</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.03612862899899483</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.03106196783483028</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.03565936908125877</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.03796902298927307</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>0.03045325540006161</v>
       </c>
+      <c r="B10" t="n">
+        <v>0.03217586502432823</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0337996631860733</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.03140239417552948</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.03363600000739098</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.03216956183314323</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.02785801514983177</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.04037057980895042</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.03436810523271561</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.02951305918395519</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.03348608687520027</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.03178960829973221</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>0.02852308750152588</v>
       </c>
+      <c r="B11" t="n">
+        <v>0.03107269108295441</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.02924484945833683</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.03067612834274769</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.03222093358635902</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.02935073524713516</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.02539283409714699</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.03544637560844421</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.03336072340607643</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.02829466015100479</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.03256680443882942</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.03040699474513531</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>0.02807699516415596</v>
       </c>
+      <c r="B12" t="n">
+        <v>0.02922134846448898</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.02842313796281815</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.02867592126131058</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.02961232513189316</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.02715164795517921</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.02289757877588272</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.03356698527932167</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.03176772221922874</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.02704126201570034</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.03029556572437286</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.02873291075229645</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>0.02702027186751366</v>
       </c>
+      <c r="B13" t="n">
+        <v>0.02780522778630257</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.02500544860959053</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.02766196615993977</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.02873736806213856</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.02511109225451946</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.02184286899864674</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.03063421696424484</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.03054765798151493</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.02633400075137615</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.02844447828829288</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.02710217051208019</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>0.02491737902164459</v>
       </c>
+      <c r="B14" t="n">
+        <v>0.02683926746249199</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.02337374724447727</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.02493531815707684</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.02535893395543098</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0226706899702549</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.02146085351705551</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.02881429903209209</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.02867836877703667</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.02497756294906139</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.02572961524128914</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.02580254897475243</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>0.02320364490151405</v>
       </c>
+      <c r="B15" t="n">
+        <v>0.02494245581328869</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.02189086936414242</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.02439107745885849</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.02279150299727917</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.02253715880215168</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.02052129991352558</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.02553158067166805</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0279552023857832</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.02401316165924072</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.02428794652223587</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.02500148117542267</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>0.02190515212714672</v>
       </c>
+      <c r="B16" t="n">
+        <v>0.02391288802027702</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.02106943167746067</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.02254328317940235</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.02250942774116993</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.02074809744954109</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.01955326274037361</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.02184589393436909</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.02610619552433491</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.02301144599914551</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.02337499894201756</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.0223133247345686</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>0.02124162018299103</v>
       </c>
+      <c r="B17" t="n">
+        <v>0.02319941483438015</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.02081485651433468</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.02147139236330986</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.02183237671852112</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.01988231018185616</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.01684893108904362</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.02093236893415451</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.02508015558123589</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.02246208302676678</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.02259283512830734</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.02184979617595673</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>0.02036030404269695</v>
       </c>
+      <c r="B18" t="n">
+        <v>0.0227432232350111</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.02015852555632591</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.02110410295426846</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.02021206542849541</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.01846012659370899</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.01596915535628796</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.0201007816940546</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.0227826926857233</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.02163539826869965</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.02051719836890697</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.02118591032922268</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>0.02018691785633564</v>
       </c>
+      <c r="B19" t="n">
+        <v>0.02103416062891483</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.01977603323757648</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.01932637393474579</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0196241233497858</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.01783558167517185</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.01298952847719193</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.01823626831173897</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.02228694595396519</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.02075069956481457</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.02035099826753139</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.01980512589216232</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>0.01973873563110828</v>
       </c>
+      <c r="B20" t="n">
+        <v>0.02032262086868286</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.01846689358353615</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.01848668232560158</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.01887455396354198</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.01653555408120155</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.01155384723097086</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.01792440563440323</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.02138125337660313</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.02038607001304626</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.01885040290653706</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.01910353265702724</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>0.01876218616962433</v>
       </c>
+      <c r="B21" t="n">
+        <v>0.02018962427973747</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.01784691773355007</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.01821049302816391</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.01796766184270382</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.01600257307291031</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.01108483504503965</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.01682190783321857</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.02013590559363365</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.01943310350179672</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.01864826492965221</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.01835615560412407</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>0.01819640211760998</v>
       </c>
+      <c r="B22" t="n">
+        <v>0.01846086606383324</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.01743703708052635</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.01663231290876865</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.016812888905406</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.01575429923832417</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.01045507844537497</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.01583814434707165</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.01946773193776608</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.01893092319369316</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.0175385344773531</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.01807487569749355</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>0.01778173446655273</v>
       </c>
+      <c r="B23" t="n">
+        <v>0.01779202371835709</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.01670893281698227</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.01633746363222599</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.01661964878439903</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.01452508009970188</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.009701820090413094</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.01500230841338634</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.01885665208101273</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.01752587594091892</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.01725584827363491</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.01632418297231197</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>0.01697730273008347</v>
       </c>
+      <c r="B24" t="n">
+        <v>0.01717290468513966</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0160038098692894</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.01566179841756821</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.01555501390248537</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.01309275347739458</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.008797693997621536</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.01332011260092258</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.01720346324145794</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.01685035787522793</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.01625458896160126</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.01605537161231041</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
         <v>0.01608412526547909</v>
       </c>
+      <c r="B25" t="n">
+        <v>0.01652219332754612</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.01489696279168129</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.01486706640571356</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.01497976388782263</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.0129198282957077</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.007884571328759193</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.01192096993327141</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.01693747006356716</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.01672881469130516</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.01567908748984337</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.01557675562798977</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
         <v>0.01550963707268238</v>
       </c>
+      <c r="B26" t="n">
+        <v>0.01566002517938614</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.01436190027743578</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.01406300906091928</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.01440583169460297</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.01231405232101679</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.007467464543879032</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.01152944378554821</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.01491872500628233</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.01548146829009056</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.0152316689491272</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.01515600178390741</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
         <v>0.0149554330855608</v>
       </c>
+      <c r="B27" t="n">
+        <v>0.01548685599118471</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.01367706526070833</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.01379212643951178</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.01399984303861856</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.0117089943960309</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.007290530018508434</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.009703228250145912</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.01418040785938501</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.01519561186432838</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.01493680942803621</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.014850745908916</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
         <v>0.01444342359900475</v>
       </c>
+      <c r="B28" t="n">
+        <v>0.01517082937061787</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.01327989809215069</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.01313493307679892</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.0132850157096982</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.01118162367492914</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.006380783393979073</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.00740034831687808</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.01393056008964777</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.01492695976048708</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.01443468313664198</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.01374811492860317</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
         <v>0.0137763200327754</v>
       </c>
+      <c r="B29" t="n">
+        <v>0.01474781520664692</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.01284684985876083</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.01219681557267904</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.01283936575055122</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.01095981523394585</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.005028935614973307</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.006695519667118788</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.01287753041833639</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.01409176364541054</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.01434721890836954</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.01355032157152891</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
         <v>0.01331396028399467</v>
       </c>
+      <c r="B30" t="n">
+        <v>0.01383950188755989</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.01255478523671627</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.01181857008486986</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.01244290266185999</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.009948692284524441</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.004854968748986721</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.006448370404541492</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.01220494695007801</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.0134003022685647</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.01328580174595118</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0.01279322989284992</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
         <v>0.01270310487598181</v>
       </c>
+      <c r="B31" t="n">
+        <v>0.01339646615087986</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.01184686738997698</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.01153106521815062</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.01207163464277983</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.009605774655938148</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.002992708003148437</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.005884209182113409</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.01096224598586559</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.01260247081518173</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.01308641210198402</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.01192657742649317</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
         <v>0.01257488690316677</v>
       </c>
+      <c r="B32" t="n">
+        <v>0.01315639819949865</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.01153274159878492</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.01088565215468407</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.01132851094007492</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.00909818708896637</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.002607493428513408</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.005220022518187761</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.01032471749931574</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.0121587784960866</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.01282530464231968</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.01169577892869711</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
         <v>0.01178669091314077</v>
       </c>
+      <c r="B33" t="n">
+        <v>0.01280652731657028</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.01128531713038683</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.01061777956783772</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.01121367886662483</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.008310729637742043</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.002391478745266795</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.004858801607042551</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.009802629239857197</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.01183720864355564</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.01255962438881397</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.01101966481655836</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
         <v>0.01131160091608763</v>
       </c>
+      <c r="B34" t="n">
+        <v>0.01226407196372747</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.01104246638715267</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.01032621413469315</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.01096050720661879</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.007282881997525692</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.002023163018748164</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.00428632739931345</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.00931154377758503</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.01120924483984709</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.01173003856092691</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.01055661030113697</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
         <v>0.01090616546571255</v>
       </c>
+      <c r="B35" t="n">
+        <v>0.01142692100256681</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.01076494622975588</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.009792962111532688</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.01056017354130745</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.006666788831353188</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.001532348454929888</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.00372428516857326</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.008504483848810196</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.01087468769401312</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.01117232255637646</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.01022089645266533</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
         <v>0.01021838467568159</v>
       </c>
+      <c r="B36" t="n">
+        <v>0.01095853932201862</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.009742897935211658</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.009444685652852058</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.009977223351597786</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.006295522674918175</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.001312304404564202</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.003519679186865687</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.008097585290670395</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.01055547874420881</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.01076542865484953</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.009983179159462452</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
         <v>0.0100672785192728</v>
       </c>
+      <c r="B37" t="n">
+        <v>0.01067796442657709</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.009021880105137825</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.008985619992017746</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.009791012853384018</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.005735659971833229</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.001164734829217196</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.002300574444234371</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.006964948959648609</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.01027973648160696</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.01049248781055212</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.009775313548743725</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
         <v>0.009212486445903778</v>
       </c>
+      <c r="B38" t="n">
+        <v>0.01048344094306231</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.008510870859026909</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.008110915310680866</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.009178905747830868</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.005491767544299364</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.0009115382563322783</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.001913972781039774</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.005938727408647537</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.009629174135625362</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.009802410379052162</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.008829922415316105</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
         <v>0.00871895719319582</v>
       </c>
+      <c r="B39" t="n">
+        <v>0.01010326109826565</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.008211537264287472</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.007775056641548872</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.009100472554564476</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.004677162505686283</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.0006129856337793171</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.001508488901890814</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.005145538132637739</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.008485855534672737</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.009554795920848846</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.008551166392862797</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
         <v>0.008323291316628456</v>
       </c>
+      <c r="B40" t="n">
+        <v>0.009433181956410408</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.00725780613720417</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.007445192895829678</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.00811457447707653</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.00461270660161972</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.0005292841815389693</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.001113110221922398</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.00430375337600708</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.008143170736730099</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.009382315911352634</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0.008153127506375313</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
         <v>0.007693667430430651</v>
       </c>
+      <c r="B41" t="n">
+        <v>0.008241328410804272</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.00685357628390193</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.006784769706428051</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.006850247271358967</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.003743016859516501</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.0003436076221987605</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.0009686762350611389</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.003871222957968712</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.007286067120730877</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.008344585075974464</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0.00700062932446599</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
         <v>0.006868749391287565</v>
       </c>
+      <c r="B42" t="n">
+        <v>0.007850775495171547</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.006379415281116962</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.006045238580554724</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.006685435306280851</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.003304180921986699</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.0002205764612881467</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.0005490642506629229</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.003081319620832801</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.006480575539171696</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.007556617725640535</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0.006527600344270468</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
         <v>6.274947045483884e-18</v>
+      </c>
+      <c r="B43" t="n">
+        <v>4.972525942010459e-18</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-1.126021363687919e-17</v>
+      </c>
+      <c r="D43" t="n">
+        <v>6.008814670130564e-17</v>
+      </c>
+      <c r="E43" t="n">
+        <v>4.22328443744177e-17</v>
+      </c>
+      <c r="F43" t="n">
+        <v>7.299847729956788e-17</v>
+      </c>
+      <c r="G43" t="n">
+        <v>-3.994115372222934e-17</v>
+      </c>
+      <c r="H43" t="n">
+        <v>-5.036117767706188e-17</v>
+      </c>
+      <c r="I43" t="n">
+        <v>5.625649555708853e-18</v>
+      </c>
+      <c r="J43" t="n">
+        <v>3.794644737972711e-17</v>
+      </c>
+      <c r="K43" t="n">
+        <v>7.313799289040352e-17</v>
+      </c>
+      <c r="L43" t="n">
+        <v>1.719629415031184e-17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>